<commit_message>
added column reference and column index information to dictionary
</commit_message>
<xml_diff>
--- a/data/endnote_ref-type_dictionary.xlsx
+++ b/data/endnote_ref-type_dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwroberts\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wainr\OneDrive\Documents\xlsx_to_xml_endnote\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95304C19-99ED-46BB-9DCD-2DDE01E6D69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72F5583-BC0B-44C4-893D-787C34034698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8FCD020D-F4C8-425C-8854-B3B196F9C257}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{8FCD020D-F4C8-425C-8854-B3B196F9C257}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Journal article</t>
   </si>
@@ -115,6 +115,84 @@
   </si>
   <si>
     <t>&lt;ref-type name="Government Document"&gt;46&lt;/ref-type&gt;</t>
+  </si>
+  <si>
+    <t>start_col</t>
+  </si>
+  <si>
+    <t>end_col</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>BJ</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>BK</t>
+  </si>
+  <si>
+    <t>BV</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>BW</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>EM</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>start_col_no</t>
+  </si>
+  <si>
+    <t>end_col_no</t>
   </si>
 </sst>
 </file>
@@ -466,128 +544,296 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF0F123-BAC4-4203-8835-8E46FDF7D9FF}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="55.28515625" customWidth="1"/>
-    <col min="2" max="2" width="63.42578125" customWidth="1"/>
+    <col min="1" max="1" width="55.26953125" customWidth="1"/>
+    <col min="2" max="2" width="63.40625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2">
+        <v>33</v>
+      </c>
+      <c r="F2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4">
+        <v>45</v>
+      </c>
+      <c r="F4">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5">
+        <v>45</v>
+      </c>
+      <c r="F5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6">
+        <v>105</v>
+      </c>
+      <c r="F6">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7">
+        <v>123</v>
+      </c>
+      <c r="F7">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8">
+        <v>63</v>
+      </c>
+      <c r="F8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9">
+        <v>75</v>
+      </c>
+      <c r="F9">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10">
+        <v>92</v>
+      </c>
+      <c r="F10">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12">
+        <v>24</v>
+      </c>
+      <c r="F12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13">
+        <v>143</v>
+      </c>
+      <c r="F13">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>